<commit_message>
Update expanding window estimations
</commit_message>
<xml_diff>
--- a/data/fill_history.xlsx
+++ b/data/fill_history.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Documents\GitHub\MMB_forecast_application\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\GitHub\MMB_forecast_application\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A153549-FF20-4044-97EE-B7844A4BB389}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F049C03-D084-4CD3-8833-CAA1C919150A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="90" windowWidth="12040" windowHeight="10270" xr2:uid="{F57F355C-F5B3-4FCD-B8B0-BB20AF23278A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="27900" windowHeight="14760" xr2:uid="{F57F355C-F5B3-4FCD-B8B0-BB20AF23278A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>alfred</t>
   </si>
@@ -109,6 +109,24 @@
   </si>
   <si>
     <t>rinvbf</t>
+  </si>
+  <si>
+    <t>RCOND</t>
+  </si>
+  <si>
+    <t>rcondMvQd.xlsx</t>
+  </si>
+  <si>
+    <t>rconndMvQd.xlsx</t>
+  </si>
+  <si>
+    <t>RCONND</t>
+  </si>
+  <si>
+    <t>rconsMvQd.xlsx</t>
+  </si>
+  <si>
+    <t>RCONS</t>
   </si>
 </sst>
 </file>
@@ -460,18 +478,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{055F0B5A-7436-428F-9F60-327FD85FDC05}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.90625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,7 +503,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +517,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -513,7 +531,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -527,7 +545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -541,7 +559,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -555,7 +573,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -569,7 +587,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -581,6 +599,48 @@
       </c>
       <c r="D8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>